<commit_message>
Backup folder - 2023-12-18 00:35:04
</commit_message>
<xml_diff>
--- a/АСД/РР1/Таблиці залежності часу додавання: видалення даних від кількості елементів.xlsx
+++ b/АСД/РР1/Таблиці залежності часу додавання: видалення даних від кількості елементів.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/АСД/РР1/Таблиці залежності часу додавання:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897BDAB3-0B18-E541-81CD-E35697E90919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C83AF4-363B-C945-824D-B230245BB816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="2660" windowWidth="20620" windowHeight="13260" xr2:uid="{6972E40D-22B5-9A4E-B6A5-B62665345E4E}"/>
+    <workbookView xWindow="4840" yWindow="2280" windowWidth="20620" windowHeight="13260" activeTab="1" xr2:uid="{6972E40D-22B5-9A4E-B6A5-B62665345E4E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Додавання" sheetId="1" r:id="rId1"/>
+    <sheet name="Видалення" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,19 +36,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
-    <t>Таблиці залежності часу додавання/ видалення даних від кількості елементів в структурі</t>
+    <t>Таблиця залежності часу додавання даних від кількості елементів в структурі</t>
+  </si>
+  <si>
+    <t>Таблиця залежності часу видалення даних від кількості елементів в структурі</t>
+  </si>
+  <si>
+    <t>Кількість елементів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">№ заміру </t>
+  </si>
+  <si>
+    <t>Затрачений час, од.</t>
+  </si>
+  <si>
+    <t>Системна узагальнена черга</t>
+  </si>
+  <si>
+    <t>Системна неузагальнена черга</t>
+  </si>
+  <si>
+    <t>Власний клас черги</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -62,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -70,12 +100,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -390,20 +543,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FF4CFE-0CF2-9446-AB79-56F7A7FC88EB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>51799</v>
+      </c>
+      <c r="D4" s="4">
+        <v>36993</v>
+      </c>
+      <c r="E4" s="4">
+        <v>22993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="4">
+        <v>15613</v>
+      </c>
+      <c r="D5" s="4">
+        <v>20083</v>
+      </c>
+      <c r="E5" s="4">
+        <v>26294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>50000</v>
+      </c>
+      <c r="C6" s="4">
+        <v>586180</v>
+      </c>
+      <c r="D6" s="4">
+        <v>92636</v>
+      </c>
+      <c r="E6" s="4">
+        <v>92207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="4">
+        <v>94982</v>
+      </c>
+      <c r="D7" s="4">
+        <v>311894</v>
+      </c>
+      <c r="E7" s="4">
+        <v>160529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12">
+        <v>100000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>408859</v>
+      </c>
+      <c r="D8" s="4">
+        <v>178733</v>
+      </c>
+      <c r="E8" s="4">
+        <v>160546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="4">
+        <v>585621</v>
+      </c>
+      <c r="D9" s="4">
+        <v>424912</v>
+      </c>
+      <c r="E9" s="4">
+        <v>135258</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C8DC38-3F12-A14C-83B3-83836F78F58F}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>13570</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8780</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="4">
+        <v>3215</v>
+      </c>
+      <c r="D5" s="14">
+        <v>4838</v>
+      </c>
+      <c r="E5" s="14">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <v>50000</v>
+      </c>
+      <c r="C6" s="4">
+        <v>132706</v>
+      </c>
+      <c r="D6" s="4">
+        <v>26462</v>
+      </c>
+      <c r="E6" s="4">
+        <v>39623</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="4">
+        <v>41051</v>
+      </c>
+      <c r="D7" s="4">
+        <v>19113</v>
+      </c>
+      <c r="E7" s="4">
+        <v>43789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12">
+        <v>100000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>55270</v>
+      </c>
+      <c r="D8" s="4">
+        <v>41665</v>
+      </c>
+      <c r="E8" s="4">
+        <v>75493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="4">
+        <v>42022</v>
+      </c>
+      <c r="D9" s="4">
+        <v>31162</v>
+      </c>
+      <c r="E9" s="4">
+        <v>71916</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup folder - 2023-12-20 00:19:26
</commit_message>
<xml_diff>
--- a/АСД/РР1/Таблиці залежності часу додавання: видалення даних від кількості елементів.xlsx
+++ b/АСД/РР1/Таблиці залежності часу додавання: видалення даних від кількості елементів.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/АСД/РР1/Таблиці залежності часу додавання:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C83AF4-363B-C945-824D-B230245BB816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B759557-7FAA-1E4A-BD22-657A125000A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="2280" windowWidth="20620" windowHeight="13260" activeTab="1" xr2:uid="{6972E40D-22B5-9A4E-B6A5-B62665345E4E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20620" windowHeight="13260" activeTab="1" xr2:uid="{6972E40D-22B5-9A4E-B6A5-B62665345E4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Додавання" sheetId="1" r:id="rId1"/>
@@ -201,6 +201,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -213,12 +214,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -228,7 +229,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -562,21 +562,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -591,7 +591,7 @@
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="13">
         <v>10000</v>
       </c>
       <c r="C4" s="4">
@@ -608,7 +608,7 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4">
         <v>15613</v>
       </c>
@@ -623,7 +623,7 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>50000</v>
       </c>
       <c r="C6" s="4">
@@ -640,7 +640,7 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="4">
         <v>94982</v>
       </c>
@@ -655,7 +655,7 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="13">
         <v>100000</v>
       </c>
       <c r="C8" s="4">
@@ -672,7 +672,7 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="4">
         <v>585621</v>
       </c>
@@ -685,12 +685,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -701,7 +701,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A4" sqref="A4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,21 +719,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -748,7 +748,7 @@
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="13">
         <v>10000</v>
       </c>
       <c r="C4" s="4">
@@ -765,14 +765,14 @@
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4">
         <v>3215</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="5">
         <v>4838</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="5">
         <v>12008</v>
       </c>
     </row>
@@ -780,7 +780,7 @@
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>50000</v>
       </c>
       <c r="C6" s="4">
@@ -797,7 +797,7 @@
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="4">
         <v>41051</v>
       </c>
@@ -812,7 +812,7 @@
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="13">
         <v>100000</v>
       </c>
       <c r="C8" s="4">
@@ -829,7 +829,7 @@
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="4">
         <v>42022</v>
       </c>
@@ -842,12 +842,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>